<commit_message>
New file for ASM.
</commit_message>
<xml_diff>
--- a/source/doc/Measurements4.xlsx
+++ b/source/doc/Measurements4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tixo\Work\Tikhomirov2\vi_metrics_time\source\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33661F8A-499D-468A-B1E4-3442EE611EC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F444DDA7-DD32-476A-907A-02464AF0484E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{FDD1F062-B851-49B6-886E-B3EC290E6614}"/>
   </bookViews>
@@ -706,7 +706,7 @@
   <dimension ref="A1:N61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8"/>
+      <selection activeCell="S24" sqref="S24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3145,5 +3145,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>